<commit_message>
Add Message Catalog v3 and update task backlog
Added the new Message_Catalog_v3.xlsx file and updated the Codex_Task_Backlog-20251215.xlsx document to reflect recent changes.
</commit_message>
<xml_diff>
--- a/Docs/Codex_Task_Backlog-20251215.xlsx
+++ b/Docs/Codex_Task_Backlog-20251215.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GitHub\LalaLaunchPlugin\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED1F8BB-FAB9-4CEE-9486-C24C279FF3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81455441-350D-4D1C-AF03-5697C49DED8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27285" yWindow="-21255" windowWidth="37950" windowHeight="20310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasking Order" sheetId="1" r:id="rId1"/>

</xml_diff>